<commit_message>
#103 Resolve "Automate Loading Product View Demo Data"
</commit_message>
<xml_diff>
--- a/pim/src/Pcmt/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2_attribute_groups.xlsx
+++ b/pim/src/Pcmt/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2_attribute_groups.xlsx
@@ -147,7 +147,7 @@
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>UNSPSC_CODE,GPC_CODE,ATC_CODE,ParentID,GTIN_UNIT_LEVEL,SOURCE_OF_DATA,SOURCEITEMID,LABELING,L3,COUNTRY_REGULATORY_CODE,LOCAL_REGULATORY_CODE,123</t>
+          <t>UNSPSC_CODE,GPC_CODE,ATC_CODE,ParentID,GTIN_UNIT_LEVEL,SOURCE_OF_DATA,SOURCEITEMID,LABELING,L3,COUNTRY_REGULATORY_CODE,LOCAL_REGULATORY_CODE,123,GTIN_PALLET_LEVEL,GTIN_CASE_LEVEL,GTIN_INNERPACK_LEVEL</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
@@ -169,7 +169,7 @@
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>ITEM_DESCRIPTION,SHELF_LIFE_DAYS,STORAGE_INSTRUCTIONS,MAX_TEMPERATURE_MEASURE,MIN_TEMPERATURE_MEASURE</t>
+          <t>ITEM_DESCRIPTION,SHELF_LIFE_DAYS,STORAGE_INSTRUCTIONS,MAX_TEMPERATURE_MEASURE,MIN_TEMPERATURE_MEASURE,REGULATORY_EXPIRE_DATE</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">

</xml_diff>